<commit_message>
se agrega el poder retirar del cajero automatico
</commit_message>
<xml_diff>
--- a/my_package/datos.xlsx
+++ b/my_package/datos.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torre\Desktop\Platzi\Sucursal_virtual\my_package\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7241F453-6E6B-4214-B7E2-900BC1DD9EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="users" sheetId="1" r:id="rId1"/>
+    <sheet name="machine" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>nombre</t>
   </si>
@@ -41,6 +48,12 @@
   </si>
   <si>
     <t>saldo_tarjeta_credito</t>
+  </si>
+  <si>
+    <t>saldo_giro_internacional</t>
+  </si>
+  <si>
+    <t>saldo_giro_nacional</t>
   </si>
   <si>
     <t>datacredito</t>
@@ -70,8 +83,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,13 +147,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -178,7 +199,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -212,6 +233,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -246,9 +268,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -421,14 +444,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,10 +485,16 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>66727173</v>
@@ -473,8 +502,11 @@
       <c r="C2">
         <v>1976</v>
       </c>
+      <c r="D2">
+        <v>87488652311</v>
+      </c>
       <c r="E2">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -483,15 +515,21 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>1000000</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>1116458320</v>
@@ -499,8 +537,11 @@
       <c r="C3">
         <v>1996</v>
       </c>
+      <c r="D3">
+        <v>87488652312</v>
+      </c>
       <c r="E3">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -509,15 +550,21 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>1000000</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>6500471</v>
@@ -525,8 +572,11 @@
       <c r="C4">
         <v>1979</v>
       </c>
+      <c r="D4">
+        <v>87488652313</v>
+      </c>
       <c r="E4">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -535,15 +585,21 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>1000000</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>1116280179</v>
@@ -551,8 +607,11 @@
       <c r="C5">
         <v>1234</v>
       </c>
+      <c r="D5">
+        <v>87488652314</v>
+      </c>
       <c r="E5">
-        <v>1000000</v>
+        <v>4120000</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -561,15 +620,21 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="K5">
+        <v>1000000</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>1006465176</v>
@@ -577,8 +642,11 @@
       <c r="C6">
         <v>529</v>
       </c>
+      <c r="D6">
+        <v>87488652315</v>
+      </c>
       <c r="E6">
-        <v>0</v>
+        <v>4770000</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -587,15 +655,21 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>1000000</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>1006116280</v>
@@ -603,8 +677,11 @@
       <c r="C7">
         <v>1234</v>
       </c>
+      <c r="D7">
+        <v>87488652316</v>
+      </c>
       <c r="E7">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -613,10 +690,101 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1000000</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1554F1EC-840E-43A1-B1DC-B88F4E311FA1}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>100000</v>
+      </c>
+      <c r="B1">
+        <v>50000</v>
+      </c>
+      <c r="C1">
+        <v>20000</v>
+      </c>
+      <c r="D1">
+        <v>10000</v>
+      </c>
+      <c r="E1">
+        <v>5000</v>
+      </c>
+      <c r="F1">
+        <v>2000</v>
+      </c>
+      <c r="G1">
+        <v>1000</v>
+      </c>
+      <c r="H1">
+        <v>500</v>
+      </c>
+      <c r="I1">
+        <v>200</v>
+      </c>
+      <c r="J1">
+        <v>100</v>
+      </c>
+      <c r="K1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>125</v>
+      </c>
+      <c r="B2">
+        <v>155</v>
+      </c>
+      <c r="C2">
+        <v>185</v>
+      </c>
+      <c r="D2">
+        <v>215</v>
+      </c>
+      <c r="E2">
+        <v>245</v>
+      </c>
+      <c r="F2">
+        <v>275</v>
+      </c>
+      <c r="G2">
+        <v>305</v>
+      </c>
+      <c r="H2">
+        <v>335</v>
+      </c>
+      <c r="I2">
+        <v>365</v>
+      </c>
+      <c r="J2">
+        <v>395</v>
+      </c>
+      <c r="K2">
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ya casi funciona todo
</commit_message>
<xml_diff>
--- a/my_package/datos.xlsx
+++ b/my_package/datos.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torre\Desktop\Platzi\Sucursal_virtual\my_package\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\UNIVERSIDAD\2023-2\FDP Imperativa\Proyecto\Sucursal_virtual\my_package\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7241F453-6E6B-4214-B7E2-900BC1DD9EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7135875D-34C4-4BE3-BA6E-7F50553C8A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
-    <sheet name="machine" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -447,11 +446,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +506,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -509,10 +523,10 @@
         <v>5000000</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="J2">
         <v>1000000</v>
@@ -527,7 +541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -544,10 +558,10 @@
         <v>5000000</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="J3">
         <v>1000000</v>
@@ -562,7 +576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -579,10 +593,10 @@
         <v>5000000</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="J4">
         <v>1000000</v>
@@ -597,7 +611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -611,19 +625,19 @@
         <v>87488652314</v>
       </c>
       <c r="E5">
-        <v>4120000</v>
+        <v>2949800</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>4750000</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="J5">
         <v>1000000</v>
       </c>
       <c r="K5">
-        <v>1000000</v>
+        <v>900000</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -632,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -646,13 +660,13 @@
         <v>87488652315</v>
       </c>
       <c r="E6">
-        <v>4770000</v>
+        <v>4771000</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="J6">
         <v>1000000</v>
@@ -667,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -684,10 +698,10 @@
         <v>5000000</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="J7">
         <v>1000000</v>
@@ -700,91 +714,6 @@
       </c>
       <c r="M7">
         <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1554F1EC-840E-43A1-B1DC-B88F4E311FA1}">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>100000</v>
-      </c>
-      <c r="B1">
-        <v>50000</v>
-      </c>
-      <c r="C1">
-        <v>20000</v>
-      </c>
-      <c r="D1">
-        <v>10000</v>
-      </c>
-      <c r="E1">
-        <v>5000</v>
-      </c>
-      <c r="F1">
-        <v>2000</v>
-      </c>
-      <c r="G1">
-        <v>1000</v>
-      </c>
-      <c r="H1">
-        <v>500</v>
-      </c>
-      <c r="I1">
-        <v>200</v>
-      </c>
-      <c r="J1">
-        <v>100</v>
-      </c>
-      <c r="K1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>125</v>
-      </c>
-      <c r="B2">
-        <v>155</v>
-      </c>
-      <c r="C2">
-        <v>185</v>
-      </c>
-      <c r="D2">
-        <v>215</v>
-      </c>
-      <c r="E2">
-        <v>245</v>
-      </c>
-      <c r="F2">
-        <v>275</v>
-      </c>
-      <c r="G2">
-        <v>305</v>
-      </c>
-      <c r="H2">
-        <v>335</v>
-      </c>
-      <c r="I2">
-        <v>365</v>
-      </c>
-      <c r="J2">
-        <v>395</v>
-      </c>
-      <c r="K2">
-        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>